<commit_message>
sua cap nhat dieu chuyen
</commit_message>
<xml_diff>
--- a/DowloadDieuChuyenThietBi.xlsx
+++ b/DowloadDieuChuyenThietBi.xlsx
@@ -15,81 +15,86 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="24">
   <si>
     <t>SỞ GD&amp;ĐT HƯNG YÊN</t>
   </si>
   <si>
+    <t>DANH SÁCH CÁC THIẾT BỊ ĐƯỢC SỬ DỤNG/ĐIỀU CHUYỂN</t>
+  </si>
+  <si>
     <t>TRUNG TÂM GDNN &amp; GDTX TỈNH HƯNG YÊN</t>
   </si>
   <si>
     <t>---------o0o---------</t>
   </si>
   <si>
-    <t>PHIẾU XÁC NHẬN ĐIỀU CHUYỂN</t>
-  </si>
-  <si>
     <t>Ngày: 16/04/2023</t>
   </si>
   <si>
-    <t>Số phiếu:</t>
-  </si>
-  <si>
-    <t>Tên thiết bị:</t>
+    <t>Lọc theo mã: 27</t>
+  </si>
+  <si>
+    <t>STT</t>
+  </si>
+  <si>
+    <t>Số phiếu</t>
+  </si>
+  <si>
+    <t>Ngày
+bàn giao</t>
+  </si>
+  <si>
+    <t>Mã thiết bị</t>
+  </si>
+  <si>
+    <t>Tên thiết bị</t>
+  </si>
+  <si>
+    <t>Người bàn giao</t>
+  </si>
+  <si>
+    <t>Người tiếp nhận</t>
+  </si>
+  <si>
+    <t>Nơi tiếp nhận</t>
+  </si>
+  <si>
+    <t>Ghi chú</t>
+  </si>
+  <si>
+    <t>2023-04-13</t>
   </si>
   <si>
     <t>Tấm gương của những người thành đạt</t>
   </si>
   <si>
-    <t>Mã thiết bị:</t>
-  </si>
-  <si>
-    <t>Người giao:</t>
-  </si>
-  <si>
     <t>Nguyen van A</t>
   </si>
   <si>
-    <t>Người nhận:</t>
-  </si>
-  <si>
     <t>Nguyen Van D</t>
   </si>
   <si>
-    <t>Ngày bàn giao:</t>
-  </si>
-  <si>
-    <t>2023-04-13</t>
-  </si>
-  <si>
-    <t>Tình trạng:</t>
+    <t>*Kho thiết bị dạy môn Hóa Học</t>
   </si>
   <si>
     <t>a</t>
   </si>
   <si>
-    <t>Phòng/Kho nhận:</t>
-  </si>
-  <si>
-    <t>Kho thiết bị dạy môn Hóa Học</t>
-  </si>
-  <si>
-    <t>Ngày……tháng……năm……</t>
-  </si>
-  <si>
-    <t xml:space="preserve">     Người nhận                  Người giao                     Thủ kho             Thủ trưởng đơn vị</t>
-  </si>
-  <si>
-    <t>(Ký, ghi rõ họ tên)       (Ký, ghi rõ họ tên)       (Ký, ghi rõ họ tên)      (Ký, ghi rõ họ tên)</t>
+    <t>Ngày……tháng……năm 20…</t>
+  </si>
+  <si>
+    <t>Người lập biểu</t>
+  </si>
+  <si>
+    <t>(Ký, ghi rõ họ tên)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="[$-1010000]d/m/yy;@"/>
-  </numFmts>
+  <numFmts count="0"/>
   <fonts count="5">
     <font>
       <b val="0"/>
@@ -101,15 +106,6 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <b val="1"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="13"/>
-      <color rgb="FF000000"/>
-      <name val="Times New Roman"/>
-    </font>
-    <font>
       <b val="0"/>
       <i val="0"/>
       <strike val="0"/>
@@ -119,8 +115,8 @@
       <name val="Times New Roman"/>
     </font>
     <font>
-      <b val="0"/>
-      <i val="1"/>
+      <b val="1"/>
+      <i val="0"/>
       <strike val="0"/>
       <u val="none"/>
       <sz val="13"/>
@@ -133,6 +129,15 @@
       <strike val="0"/>
       <u val="none"/>
       <sz val="15"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <b val="0"/>
+      <i val="1"/>
+      <strike val="0"/>
+      <u val="none"/>
+      <sz val="13"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
     </font>
@@ -151,53 +156,64 @@
       <patternFill patternType="none"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border/>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="2" numFmtId="49" fillId="2" borderId="0" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="2" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="2" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="4" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="2" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="3" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="2" numFmtId="49" fillId="2" borderId="0" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="2" numFmtId="164" fillId="2" borderId="0" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="2" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="2" numFmtId="49" fillId="2" borderId="0" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="4" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
+    <xf xfId="0" fontId="1" numFmtId="49" fillId="2" borderId="0" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="3" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
@@ -502,182 +518,196 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="true" defaultRowHeight="16.5" defaultColWidth="9" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="14.4" defaultColWidth="9" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" customWidth="true" style="3"/>
-    <col min="2" max="2" width="18.85546875" customWidth="true" style="3"/>
-    <col min="3" max="3" width="9" style="3"/>
-    <col min="4" max="4" width="9" style="3"/>
-    <col min="5" max="5" width="9" style="3"/>
-    <col min="6" max="6" width="12.7109375" customWidth="true" style="3"/>
-    <col min="7" max="7" width="12.42578125" customWidth="true" style="3"/>
-    <col min="8" max="8" width="9" style="3"/>
+    <col min="1" max="1" width="4.6640625" customWidth="true" style="6"/>
+    <col min="2" max="2" width="9.6640625" customWidth="true" style="6"/>
+    <col min="3" max="3" width="11.44140625" customWidth="true" style="6"/>
+    <col min="4" max="4" width="11.109375" customWidth="true" style="6"/>
+    <col min="5" max="5" width="17.44140625" customWidth="true" style="6"/>
+    <col min="6" max="6" width="21.44140625" customWidth="true" style="6"/>
+    <col min="7" max="7" width="21.44140625" customWidth="true" style="6"/>
+    <col min="8" max="8" width="21.44140625" customWidth="true" style="6"/>
+    <col min="9" max="9" width="8.33203125" customWidth="true" style="6"/>
+    <col min="10" max="10" width="9" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" customHeight="1" ht="16.5">
+    <row r="1" spans="1:10" customHeight="1" ht="18.6">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="11"/>
       <c r="C1" s="11"/>
-      <c r="D1" s="1"/>
-    </row>
-    <row r="2" spans="1:8" customHeight="1" ht="16.5">
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+    </row>
+    <row r="2" spans="1:10" customHeight="1" ht="16.5">
       <c r="A2" s="12" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" s="12"/>
       <c r="C2" s="12"/>
-      <c r="D2" s="2"/>
-    </row>
-    <row r="3" spans="1:8" customHeight="1" ht="16.5">
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+    </row>
+    <row r="3" spans="1:10" customHeight="1" ht="20.25">
       <c r="A3" s="12" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B3" s="12"/>
       <c r="C3" s="12"/>
-      <c r="D3" s="2"/>
-    </row>
-    <row r="4" spans="1:8" customHeight="1" ht="35.25">
-      <c r="A4" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-    </row>
-    <row r="5" spans="1:8" customHeight="1" ht="16.5">
-      <c r="A5" s="14" t="s">
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="14"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-    </row>
-    <row r="6" spans="1:8" customHeight="1" ht="12">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-    </row>
-    <row r="7" spans="1:8" customHeight="1" ht="18.75">
-      <c r="A7" s="3" t="s">
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+    </row>
+    <row r="4" spans="1:10" customHeight="1" ht="21">
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="F4" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="7">
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+    </row>
+    <row r="5" spans="1:10" customHeight="1" ht="18">
+      <c r="A5" s="7"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+    </row>
+    <row r="6" spans="1:10" customHeight="1" ht="33.6">
+      <c r="A6" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="I6" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" customHeight="1" ht="33.6">
+      <c r="A7" s="9">
+        <v>1</v>
+      </c>
+      <c r="B7" s="9">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" customHeight="1" ht="18.75">
-      <c r="A8" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" customHeight="1" ht="18.75">
-      <c r="A9" s="3" t="s">
+      <c r="C7" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="9">
         <v>8</v>
       </c>
-      <c r="B9" s="7">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" customHeight="1" ht="18.75">
-      <c r="A10" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" customHeight="1" ht="18.75">
-      <c r="A11" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" customHeight="1" ht="18.75">
-      <c r="A12" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" customHeight="1" ht="18.75">
-      <c r="A13" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" s="4" t="s">
+      <c r="E7" s="9" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" customHeight="1" ht="18.75">
-      <c r="A14" s="3" t="s">
+      <c r="F7" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="G7" s="9" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" customHeight="1" ht="12"/>
-    <row r="16" spans="1:8" customHeight="1" ht="19.5">
-      <c r="D16" s="6" t="s">
+      <c r="H7" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-    </row>
-    <row r="17" spans="1:8" customHeight="1" ht="16.5">
-      <c r="A17" s="9" t="s">
+      <c r="I7" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="10"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
-    </row>
-    <row r="18" spans="1:8" customHeight="1" ht="16.5">
-      <c r="A18" s="10" t="s">
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="5"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="3"/>
+    </row>
+    <row r="9" spans="1:10" customHeight="1" ht="19.5">
+      <c r="A9" s="5"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="10"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
+      <c r="H9" s="11"/>
+    </row>
+    <row r="10" spans="1:10" customHeight="1" ht="19.5">
+      <c r="G10" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="H10" s="11"/>
+    </row>
+    <row r="11" spans="1:10" customHeight="1" ht="19.5">
+      <c r="G11" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="H11" s="10"/>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
   <mergeCells>
-    <mergeCell ref="A17:F17"/>
-    <mergeCell ref="A18:F18"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A4:F4"/>
-    <mergeCell ref="A5:F5"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="F3:I3"/>
+    <mergeCell ref="F4:I4"/>
   </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true"/>
-  <pageMargins left="0.95" right="0.56" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" scale="100" fitToHeight="1" fitToWidth="1"/>
+  <pageMargins left="0.43" right="0.45" top="0.6" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" scale="100" fitToHeight="1" fitToWidth="1"/>
   <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
     <oddHeader/>
     <oddFooter/>

</xml_diff>